<commit_message>
Added method to delete file after the screenshot added in the pdf page
Files.deleteIfExists(Paths.get(pathToScreenshot) );
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1053,7 +1053,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add method to delete the screenshot
Added:
Files.deleteIfExists(Paths.get(pathToScreenshot));
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -688,7 +688,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Refactor - Review (Architecture Logic)
Refactor - Review (Architecture Logic)
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -688,7 +688,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Deleted the file environment.properties
Deleted the file environment.properties
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1053,7 +1053,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the code to created a folder using the test name String, to organize better the pdf report files.
Added the code to created a folder using the test name String, to organize better the pdf report files.
File file = new File(".//src//main//report//"+textTestCase);
file.mkdir();
String pathtoFolder=file.getAbsolutePath().toString();
PdfWriter.getInstance(document, new FileOutputStream((pathtoFolder+"//"+textTestCase+""+"_alpha-sense-evidencia.pdf")));
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Test_PageCreateAnAccountError</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refactor - PDF report for Downloaded invoice
Refactor - PDF report for Downloaded invoice
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -3,23 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:801_{A4C2A3D1-BA74-4A4D-91AE-F80FD0AD9757}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E77960C4-FA93-4B2B-88D1-812AA1B31DA5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="2" windowHeight="13224" windowWidth="23304" xWindow="384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="384"/>
+    <workbookView activeTab="1" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Test_PageLogin" r:id="rId1" sheetId="7"/>
-    <sheet name="Test_PageCreateAnAccount" r:id="rId2" sheetId="8"/>
-    <sheet name="Test_PageMyAccountSearchClothes" r:id="rId3" sheetId="9"/>
+    <sheet name="sheetCreateAccount" r:id="rId2" sheetId="8"/>
+    <sheet name="sheetSearchClothes" r:id="rId3" sheetId="9"/>
     <sheet name="sheetOrderShipClothes" r:id="rId4" sheetId="10"/>
+    <sheet name="Test_DownloadPDFInvoice" r:id="rId5" sheetId="11"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:N9"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>ExpectedResponse</t>
   </si>
   <si>
-    <t>Account Created</t>
-  </si>
-  <si>
     <t>Failed To Create Account</t>
   </si>
   <si>
@@ -159,12 +156,6 @@
     <t>SetEmail</t>
   </si>
   <si>
-    <t>alskfjasdf@gmail.com</t>
-  </si>
-  <si>
-    <t>a23342@gmail.com</t>
-  </si>
-  <si>
     <t>qwertyuio</t>
   </si>
   <si>
@@ -177,10 +168,13 @@
     <t>Test_PageMyAccountSearchClothes</t>
   </si>
   <si>
+    <t>Test_PageMyAccountOrderShipClothes</t>
+  </si>
+  <si>
     <t>Test_PageCreateAnAccountError</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>Test_DownloadPDFInvoice</t>
   </si>
 </sst>
 </file>
@@ -188,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +219,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,7 +284,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -301,6 +302,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hiperligação" xfId="1"/>
@@ -642,7 +644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91728534-B49C-467B-BE81-CB63041BE581}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -676,7 +680,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -691,12 +695,12 @@
         <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -711,7 +715,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -734,13 +738,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0565ED-5EA1-41B2-AB48-F3BD1B1DE068}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
@@ -777,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>35</v>
@@ -821,7 +825,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -835,11 +839,9 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="F2" s="11"/>
       <c r="G2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>22</v>
@@ -863,7 +865,7 @@
         <v>28</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="5">
         <v>123456789</v>
@@ -872,13 +874,13 @@
         <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -892,11 +894,9 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="F3" s="11"/>
       <c r="G3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>30</v>
@@ -920,7 +920,7 @@
         <v>28</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" s="5">
         <v>123456789</v>
@@ -929,7 +929,7 @@
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="S3" s="5"/>
     </row>
@@ -939,28 +939,26 @@
   </sheetData>
   <hyperlinks>
     <hyperlink display="carloscgta@gmail.com" r:id="rId1" ref="B2" xr:uid="{CB0965AE-63A9-4312-B445-F2F2AA9CB773}"/>
-    <hyperlink r:id="rId2" ref="F2" xr:uid="{CDF39BD0-C94B-4E48-B7D6-2495A9773564}"/>
-    <hyperlink r:id="rId3" ref="Q2" xr:uid="{161FAB1D-C582-4AA8-A8A5-CD77C90AC59C}"/>
-    <hyperlink display="carloscgta@gmail.com" r:id="rId4" ref="B3" xr:uid="{1DCA593C-0A08-4CAC-904A-080A628A9E62}"/>
-    <hyperlink r:id="rId5" ref="Q3" xr:uid="{698E0C43-F739-42A9-A862-05CDA9111E0C}"/>
-    <hyperlink r:id="rId6" ref="F3" xr:uid="{F0910E50-0B60-4DE0-8271-60C921B4A451}"/>
+    <hyperlink r:id="rId2" ref="Q2" xr:uid="{161FAB1D-C582-4AA8-A8A5-CD77C90AC59C}"/>
+    <hyperlink display="carloscgta@gmail.com" r:id="rId3" ref="B3" xr:uid="{1DCA593C-0A08-4CAC-904A-080A628A9E62}"/>
+    <hyperlink r:id="rId4" ref="Q3" xr:uid="{698E0C43-F739-42A9-A862-05CDA9111E0C}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId7"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98AB0D2-000A-4AA4-840B-AE69750F0C19}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.109375" collapsed="true"/>
@@ -971,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -985,10 +983,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -999,30 +997,27 @@
       <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="carloscgta@gmail.com" r:id="rId1" ref="B2" xr:uid="{28006B2B-8ED0-47B4-AFCB-896E8BB99A03}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1571D06B-4CC2-43FC-BD8A-CE1875325B3D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1030,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
@@ -1044,10 +1039,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1056,14 +1051,109 @@
         <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="carloscgta@gmail.com" r:id="rId1" ref="B2" xr:uid="{2FC36240-7D4A-4BC7-A85F-05F9D4D5FD97}"/>
+    <hyperlink display="carloscgta@gmail.com" r:id="rId2" ref="B3" xr:uid="{A02440E1-D4B3-4ECC-BECA-B4A81A49EBBD}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADBA3C8-5E67-4AF6-A3FE-E0C67534D543}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink display="carloscgta@gmail.com" r:id="rId1" ref="B2" xr:uid="{AAC5457C-DC67-4D5E-8E1E-9002D3CC882E}"/>
+    <hyperlink display="carloscgta@gmail.com" r:id="rId2" ref="B3" xr:uid="{E307A699-6EEB-4239-9038-5668F734D74E}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>